<commit_message>
upload: campinas, sexo masculino 2010-2020
</commit_message>
<xml_diff>
--- a/analysis_Campinas/campinas_tabnet/fem/cps2010_fem_c.xlsx
+++ b/analysis_Campinas/campinas_tabnet/fem/cps2010_fem_c.xlsx
@@ -569,7 +569,7 @@
         <v>8</v>
       </c>
       <c r="W2" t="n">
-        <v>2682</v>
+        <v>894</v>
       </c>
     </row>
     <row r="3">
@@ -640,7 +640,7 @@
         <v>3</v>
       </c>
       <c r="W3" t="n">
-        <v>297</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4">
@@ -711,7 +711,7 @@
         <v>7</v>
       </c>
       <c r="W4" t="n">
-        <v>1476</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5">
@@ -782,7 +782,7 @@
         <v>2</v>
       </c>
       <c r="W5" t="n">
-        <v>420</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6">
@@ -853,7 +853,7 @@
         <v>1</v>
       </c>
       <c r="W6" t="n">
-        <v>1767</v>
+        <v>589</v>
       </c>
     </row>
     <row r="7">
@@ -924,7 +924,7 @@
         <v>6</v>
       </c>
       <c r="W7" t="n">
-        <v>2235</v>
+        <v>745</v>
       </c>
     </row>
     <row r="8">
@@ -995,7 +995,7 @@
         <v>27</v>
       </c>
       <c r="W8" t="n">
-        <v>8877</v>
+        <v>2959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>